<commit_message>
changing the case study names to allow RMSE bangladesh to work
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/test_results_Bangladesh.xlsx
+++ b/heliostrome/jip_project/results/test_results_Bangladesh.xlsx
@@ -552,16 +552,16 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[35, 35, 35, 35]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
@@ -573,14 +573,14 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>[26]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Summer Tomato - Drip (Gazipur)</t>
+          <t>Summer Tomato - Drip (Gazipur) SD(1)</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -611,16 +611,16 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[35, 35, 35, 35]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
@@ -632,14 +632,14 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>[26]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Summer Tomato - Drip (Gazipur)</t>
+          <t>Summer Tomato - Drip (Gazipur) SD(2)</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -670,16 +670,16 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[35, 35, 35, 35]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
@@ -691,14 +691,14 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>[26]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Winter Tomato - Drip (Gazipur)</t>
+          <t>Winter Tomato - Drip (Gazipur) (Y1)</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -729,16 +729,16 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>[35, 35, 35, 35]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L5" t="inlineStr"/>
@@ -750,14 +750,14 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>[26]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Winter Tomato - Furrow (Gazipur)</t>
+          <t>Winter Tomato - Furrow (Gazipur) (SD1)</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -788,16 +788,16 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>[35, 35, 35, 35]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L6" t="inlineStr"/>
@@ -809,14 +809,14 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>[26]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Winter Tomato - Drip (Gazipur)</t>
+          <t>Winter Tomato - Drip (Gazipur) (Y2)</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -847,16 +847,16 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>[35, 35, 35, 35]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L7" t="inlineStr"/>
@@ -868,14 +868,14 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>[26]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Winter Tomato - Furrow (Gazipur)</t>
+          <t>Winter Tomato - Furrow (Gazipur) (SD2)</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -906,16 +906,16 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>[35, 35, 35, 35]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L8" t="inlineStr"/>
@@ -927,7 +927,7 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>[26]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -965,16 +965,16 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>[33, 33, 33, 33]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L9" t="inlineStr"/>
@@ -986,7 +986,7 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>[22]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -1024,16 +1024,16 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>[33, 33, 33, 33]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L10" t="inlineStr"/>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>[22]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -1083,16 +1083,16 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L11" t="inlineStr"/>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>[22]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -1142,16 +1142,16 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L12" t="inlineStr"/>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>[22]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -1201,16 +1201,16 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>[32, 32, 32, 32]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L13" t="inlineStr"/>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>[22]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -1262,16 +1262,16 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>[32, 32, 32, 32]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L14" t="inlineStr"/>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>[22]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -1323,16 +1323,16 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>[100, 100, 100, 100]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L15" t="inlineStr"/>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>[26]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -1382,16 +1382,16 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>[100, 100, 100, 100]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L16" t="inlineStr"/>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>[50]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -1441,16 +1441,16 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>[100, 100, 100, 100]</t>
+          <t>[0. 0. 0. 0.]</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Pct</t>
+          <t>Prop</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>[41]</t>
+          <t>['FC']</t>
         </is>
       </c>
     </row>
@@ -1543,10 +1543,10 @@
         <v>285</v>
       </c>
       <c r="F2" t="n">
-        <v>8.252035301011807</v>
+        <v>8.254857057132657</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>9.403343776218572</v>
       </c>
     </row>
     <row r="3">
@@ -1570,10 +1570,10 @@
         <v>650</v>
       </c>
       <c r="F3" t="n">
-        <v>8.265331847337418</v>
+        <v>8.277729612791207</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>113.0564444647878</v>
       </c>
     </row>
     <row r="4">
@@ -1597,10 +1597,10 @@
         <v>1016</v>
       </c>
       <c r="F4" t="n">
-        <v>8.331373152267158</v>
+        <v>8.331522595200999</v>
       </c>
       <c r="G4" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1624,16 +1624,16 @@
         <v>1381</v>
       </c>
       <c r="F5" t="n">
-        <v>8.329031300172565</v>
+        <v>8.348821793627463</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>23.32236107832408</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Summer Tomato - Drip (Gazipur)</t>
+          <t>Summer Tomato - Drip (Gazipur) SD(1)</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1651,16 +1651,16 @@
         <v>285</v>
       </c>
       <c r="F6" t="n">
-        <v>8.252035301011807</v>
+        <v>8.254857057132657</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>9.403343776218572</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Summer Tomato - Drip (Gazipur)</t>
+          <t>Summer Tomato - Drip (Gazipur) SD(1)</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1678,16 +1678,16 @@
         <v>650</v>
       </c>
       <c r="F7" t="n">
-        <v>8.265331847337418</v>
+        <v>8.277729612791207</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>113.0564444647878</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Summer Tomato - Drip (Gazipur)</t>
+          <t>Summer Tomato - Drip (Gazipur) SD(1)</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1705,16 +1705,16 @@
         <v>1016</v>
       </c>
       <c r="F8" t="n">
-        <v>8.331373152267158</v>
+        <v>8.331522595200999</v>
       </c>
       <c r="G8" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Summer Tomato - Drip (Gazipur)</t>
+          <t>Summer Tomato - Drip (Gazipur) SD(1)</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1732,16 +1732,16 @@
         <v>1381</v>
       </c>
       <c r="F9" t="n">
-        <v>8.329031300172565</v>
+        <v>8.348821793627463</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>23.32236107832408</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Summer Tomato - Drip (Gazipur)</t>
+          <t>Summer Tomato - Drip (Gazipur) SD(2)</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1759,16 +1759,16 @@
         <v>285</v>
       </c>
       <c r="F10" t="n">
-        <v>8.252035301011807</v>
+        <v>8.254857057132657</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>9.403343776218572</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Summer Tomato - Drip (Gazipur)</t>
+          <t>Summer Tomato - Drip (Gazipur) SD(2)</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1786,16 +1786,16 @@
         <v>650</v>
       </c>
       <c r="F11" t="n">
-        <v>8.265331847337418</v>
+        <v>8.277729612791207</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>113.0564444647878</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Summer Tomato - Drip (Gazipur)</t>
+          <t>Summer Tomato - Drip (Gazipur) SD(2)</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -1813,16 +1813,16 @@
         <v>1016</v>
       </c>
       <c r="F12" t="n">
-        <v>8.331373152267158</v>
+        <v>8.331522595200999</v>
       </c>
       <c r="G12" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Summer Tomato - Drip (Gazipur)</t>
+          <t>Summer Tomato - Drip (Gazipur) SD(2)</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1840,16 +1840,16 @@
         <v>1381</v>
       </c>
       <c r="F13" t="n">
-        <v>8.329031300172565</v>
+        <v>8.348821793627463</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>23.32236107832408</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Winter Tomato - Drip (Gazipur)</t>
+          <t>Winter Tomato - Drip (Gazipur) (Y1)</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1867,16 +1867,16 @@
         <v>446</v>
       </c>
       <c r="F14" t="n">
-        <v>5.799594592429121</v>
+        <v>8.152824574119061</v>
       </c>
       <c r="G14" t="n">
-        <v>625</v>
+        <v>623.1157872657654</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Winter Tomato - Drip (Gazipur)</t>
+          <t>Winter Tomato - Drip (Gazipur) (Y1)</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1894,16 +1894,16 @@
         <v>811</v>
       </c>
       <c r="F15" t="n">
-        <v>5.724272415628232</v>
+        <v>8.22490587834845</v>
       </c>
       <c r="G15" t="n">
-        <v>600</v>
+        <v>559.2473247716565</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Winter Tomato - Drip (Gazipur)</t>
+          <t>Winter Tomato - Drip (Gazipur) (Y1)</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1921,16 +1921,16 @@
         <v>1177</v>
       </c>
       <c r="F16" t="n">
-        <v>5.425883008718891</v>
+        <v>8.26548949529284</v>
       </c>
       <c r="G16" t="n">
-        <v>575</v>
+        <v>554.46743171663</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Winter Tomato - Furrow (Gazipur)</t>
+          <t>Winter Tomato - Furrow (Gazipur) (SD1)</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1948,16 +1948,16 @@
         <v>446</v>
       </c>
       <c r="F17" t="n">
-        <v>5.799594592429121</v>
+        <v>8.152824574119061</v>
       </c>
       <c r="G17" t="n">
-        <v>625</v>
+        <v>623.1157872657654</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Winter Tomato - Furrow (Gazipur)</t>
+          <t>Winter Tomato - Furrow (Gazipur) (SD1)</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1975,16 +1975,16 @@
         <v>811</v>
       </c>
       <c r="F18" t="n">
-        <v>5.724272415628232</v>
+        <v>8.22490587834845</v>
       </c>
       <c r="G18" t="n">
-        <v>600</v>
+        <v>559.2473247716565</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Winter Tomato - Furrow (Gazipur)</t>
+          <t>Winter Tomato - Furrow (Gazipur) (SD1)</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -2002,16 +2002,16 @@
         <v>1177</v>
       </c>
       <c r="F19" t="n">
-        <v>5.425883008718891</v>
+        <v>8.26548949529284</v>
       </c>
       <c r="G19" t="n">
-        <v>575</v>
+        <v>554.46743171663</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Winter Tomato - Drip (Gazipur)</t>
+          <t>Winter Tomato - Drip (Gazipur) (Y2)</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -2029,16 +2029,16 @@
         <v>446</v>
       </c>
       <c r="F20" t="n">
-        <v>5.799594592429121</v>
+        <v>8.152824574119061</v>
       </c>
       <c r="G20" t="n">
-        <v>625</v>
+        <v>623.1157872657654</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Winter Tomato - Drip (Gazipur)</t>
+          <t>Winter Tomato - Drip (Gazipur) (Y2)</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -2056,16 +2056,16 @@
         <v>811</v>
       </c>
       <c r="F21" t="n">
-        <v>5.724272415628232</v>
+        <v>8.22490587834845</v>
       </c>
       <c r="G21" t="n">
-        <v>600</v>
+        <v>559.2473247716565</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Winter Tomato - Drip (Gazipur)</t>
+          <t>Winter Tomato - Drip (Gazipur) (Y2)</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -2083,16 +2083,16 @@
         <v>1177</v>
       </c>
       <c r="F22" t="n">
-        <v>5.425883008718891</v>
+        <v>8.26548949529284</v>
       </c>
       <c r="G22" t="n">
-        <v>575</v>
+        <v>554.46743171663</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Winter Tomato - Furrow (Gazipur)</t>
+          <t>Winter Tomato - Furrow (Gazipur) (SD2)</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -2110,16 +2110,16 @@
         <v>446</v>
       </c>
       <c r="F23" t="n">
-        <v>5.799594592429121</v>
+        <v>8.152824574119061</v>
       </c>
       <c r="G23" t="n">
-        <v>625</v>
+        <v>623.1157872657654</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Winter Tomato - Furrow (Gazipur)</t>
+          <t>Winter Tomato - Furrow (Gazipur) (SD2)</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -2137,16 +2137,16 @@
         <v>811</v>
       </c>
       <c r="F24" t="n">
-        <v>5.724272415628232</v>
+        <v>8.22490587834845</v>
       </c>
       <c r="G24" t="n">
-        <v>600</v>
+        <v>559.2473247716565</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Winter Tomato - Furrow (Gazipur)</t>
+          <t>Winter Tomato - Furrow (Gazipur) (SD2)</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -2164,10 +2164,10 @@
         <v>1177</v>
       </c>
       <c r="F25" t="n">
-        <v>5.425883008718891</v>
+        <v>8.26548949529284</v>
       </c>
       <c r="G25" t="n">
-        <v>575</v>
+        <v>554.46743171663</v>
       </c>
     </row>
     <row r="26">
@@ -2191,10 +2191,10 @@
         <v>416</v>
       </c>
       <c r="F26" t="n">
-        <v>2.199050389369717</v>
+        <v>8.116140477194804</v>
       </c>
       <c r="G26" t="n">
-        <v>324.6294128218001</v>
+        <v>493.7507086671172</v>
       </c>
     </row>
     <row r="27">
@@ -2218,10 +2218,10 @@
         <v>781</v>
       </c>
       <c r="F27" t="n">
-        <v>3.619606235631393</v>
+        <v>8.151121539390644</v>
       </c>
       <c r="G27" t="n">
-        <v>350</v>
+        <v>454.1084447394541</v>
       </c>
     </row>
     <row r="28">
@@ -2245,10 +2245,10 @@
         <v>1147</v>
       </c>
       <c r="F28" t="n">
-        <v>1.494692662904003</v>
+        <v>8.188330610980953</v>
       </c>
       <c r="G28" t="n">
-        <v>275</v>
+        <v>440.1297618031599</v>
       </c>
     </row>
     <row r="29">
@@ -2272,10 +2272,10 @@
         <v>416</v>
       </c>
       <c r="F29" t="n">
-        <v>2.199050389369717</v>
+        <v>8.116140477194804</v>
       </c>
       <c r="G29" t="n">
-        <v>324.6294128218001</v>
+        <v>493.7507086671172</v>
       </c>
     </row>
     <row r="30">
@@ -2299,10 +2299,10 @@
         <v>781</v>
       </c>
       <c r="F30" t="n">
-        <v>3.619606235631393</v>
+        <v>8.151121539390644</v>
       </c>
       <c r="G30" t="n">
-        <v>350</v>
+        <v>454.1084447394541</v>
       </c>
     </row>
     <row r="31">
@@ -2326,10 +2326,10 @@
         <v>1147</v>
       </c>
       <c r="F31" t="n">
-        <v>1.494692662904003</v>
+        <v>8.188330610980953</v>
       </c>
       <c r="G31" t="n">
-        <v>275</v>
+        <v>440.1297618031599</v>
       </c>
     </row>
     <row r="32">
@@ -2353,10 +2353,10 @@
         <v>429</v>
       </c>
       <c r="F32" t="n">
-        <v>1.75629891650748</v>
+        <v>8.149854613466564</v>
       </c>
       <c r="G32" t="n">
-        <v>325</v>
+        <v>521.722267415854</v>
       </c>
     </row>
     <row r="33">
@@ -2380,10 +2380,10 @@
         <v>794</v>
       </c>
       <c r="F33" t="n">
-        <v>1.404878119678743</v>
+        <v>8.18529050471156</v>
       </c>
       <c r="G33" t="n">
-        <v>275</v>
+        <v>489.5130707729779</v>
       </c>
     </row>
     <row r="34">
@@ -2407,10 +2407,10 @@
         <v>1160</v>
       </c>
       <c r="F34" t="n">
-        <v>1.775297960730243</v>
+        <v>8.234694634428431</v>
       </c>
       <c r="G34" t="n">
-        <v>300</v>
+        <v>475.1946539421569</v>
       </c>
     </row>
     <row r="35">
@@ -2434,10 +2434,10 @@
         <v>429</v>
       </c>
       <c r="F35" t="n">
-        <v>1.75629891650748</v>
+        <v>8.149854613466564</v>
       </c>
       <c r="G35" t="n">
-        <v>325</v>
+        <v>521.722267415854</v>
       </c>
     </row>
     <row r="36">
@@ -2461,10 +2461,10 @@
         <v>794</v>
       </c>
       <c r="F36" t="n">
-        <v>1.404878119678743</v>
+        <v>8.18529050471156</v>
       </c>
       <c r="G36" t="n">
-        <v>275</v>
+        <v>489.5130707729779</v>
       </c>
     </row>
     <row r="37">
@@ -2488,10 +2488,10 @@
         <v>1160</v>
       </c>
       <c r="F37" t="n">
-        <v>1.775297960730243</v>
+        <v>8.234694634428431</v>
       </c>
       <c r="G37" t="n">
-        <v>300</v>
+        <v>475.1946539421569</v>
       </c>
     </row>
     <row r="38">
@@ -2515,10 +2515,10 @@
         <v>392</v>
       </c>
       <c r="F38" t="n">
-        <v>6.219102643765745</v>
+        <v>8.160466078310424</v>
       </c>
       <c r="G38" t="n">
-        <v>375</v>
+        <v>396.6686663362698</v>
       </c>
     </row>
     <row r="39">
@@ -2542,10 +2542,10 @@
         <v>757</v>
       </c>
       <c r="F39" t="n">
-        <v>2.667879848391237</v>
+        <v>8.145782130926303</v>
       </c>
       <c r="G39" t="n">
-        <v>275</v>
+        <v>420.0252606894488</v>
       </c>
     </row>
     <row r="40">
@@ -2569,10 +2569,10 @@
         <v>1123</v>
       </c>
       <c r="F40" t="n">
-        <v>1.910364104782561</v>
+        <v>8.159362150667588</v>
       </c>
       <c r="G40" t="n">
-        <v>275</v>
+        <v>439.1301208475674</v>
       </c>
     </row>
     <row r="41">
@@ -2596,10 +2596,10 @@
         <v>392</v>
       </c>
       <c r="F41" t="n">
-        <v>6.219102643765745</v>
+        <v>8.160466078310424</v>
       </c>
       <c r="G41" t="n">
-        <v>375</v>
+        <v>396.6686663362698</v>
       </c>
     </row>
     <row r="42">
@@ -2623,10 +2623,10 @@
         <v>757</v>
       </c>
       <c r="F42" t="n">
-        <v>2.667879848391237</v>
+        <v>8.145782130926303</v>
       </c>
       <c r="G42" t="n">
-        <v>275</v>
+        <v>420.0252606894488</v>
       </c>
     </row>
     <row r="43">
@@ -2650,10 +2650,10 @@
         <v>1123</v>
       </c>
       <c r="F43" t="n">
-        <v>1.910364104782561</v>
+        <v>8.159362150667588</v>
       </c>
       <c r="G43" t="n">
-        <v>275</v>
+        <v>439.1301208475674</v>
       </c>
     </row>
     <row r="44">
@@ -2677,10 +2677,10 @@
         <v>522</v>
       </c>
       <c r="F44" t="n">
-        <v>10.38090308910392</v>
+        <v>10.98050787905975</v>
       </c>
       <c r="G44" t="n">
-        <v>1172.759181615765</v>
+        <v>789.0064062777657</v>
       </c>
     </row>
     <row r="45">
@@ -2704,10 +2704,10 @@
         <v>887</v>
       </c>
       <c r="F45" t="n">
-        <v>10.41834274183897</v>
+        <v>11.02363371829305</v>
       </c>
       <c r="G45" t="n">
-        <v>1203.58392751751</v>
+        <v>759.754732053014</v>
       </c>
     </row>
     <row r="46">
@@ -2731,10 +2731,10 @@
         <v>1253</v>
       </c>
       <c r="F46" t="n">
-        <v>10.46257201215936</v>
+        <v>11.07063181320648</v>
       </c>
       <c r="G46" t="n">
-        <v>1152.695525218605</v>
+        <v>774.2887670850631</v>
       </c>
     </row>
     <row r="47">
@@ -2758,10 +2758,10 @@
         <v>131</v>
       </c>
       <c r="F47" t="n">
-        <v>6.989670147640976</v>
+        <v>6.685001310430317</v>
       </c>
       <c r="G47" t="n">
-        <v>722.8977391671099</v>
+        <v>635.4148958486646</v>
       </c>
     </row>
     <row r="48">
@@ -2785,10 +2785,10 @@
         <v>496</v>
       </c>
       <c r="F48" t="n">
-        <v>7.015346729218368</v>
+        <v>6.663760289770972</v>
       </c>
       <c r="G48" t="n">
-        <v>689.147681439479</v>
+        <v>576.7753762708826</v>
       </c>
     </row>
     <row r="49">
@@ -2812,10 +2812,10 @@
         <v>861</v>
       </c>
       <c r="F49" t="n">
-        <v>7.043660632884428</v>
+        <v>6.665636245753939</v>
       </c>
       <c r="G49" t="n">
-        <v>687.9765759548468</v>
+        <v>569.842385873952</v>
       </c>
     </row>
     <row r="50">
@@ -2839,10 +2839,10 @@
         <v>1227</v>
       </c>
       <c r="F50" t="n">
-        <v>7.082644536901525</v>
+        <v>6.818304607624293</v>
       </c>
       <c r="G50" t="n">
-        <v>674.9028563351791</v>
+        <v>586.3869258097915</v>
       </c>
     </row>
     <row r="51">
@@ -2866,10 +2866,10 @@
         <v>137</v>
       </c>
       <c r="F51" t="n">
-        <v>6.989670147640976</v>
+        <v>6.691117006220352</v>
       </c>
       <c r="G51" t="n">
-        <v>696.9296587599061</v>
+        <v>566.12726644269</v>
       </c>
     </row>
     <row r="52">
@@ -2893,10 +2893,10 @@
         <v>502</v>
       </c>
       <c r="F52" t="n">
-        <v>7.015211013062076</v>
+        <v>6.643738165280067</v>
       </c>
       <c r="G52" t="n">
-        <v>698.2311625269382</v>
+        <v>525.945710868946</v>
       </c>
     </row>
     <row r="53">
@@ -2920,10 +2920,10 @@
         <v>867</v>
       </c>
       <c r="F53" t="n">
-        <v>7.047831954663301</v>
+        <v>6.671830562414732</v>
       </c>
       <c r="G53" t="n">
-        <v>665.171884249018</v>
+        <v>506.6232797723603</v>
       </c>
     </row>
     <row r="54">
@@ -2947,10 +2947,10 @@
         <v>1233</v>
       </c>
       <c r="F54" t="n">
-        <v>7.08299744934908</v>
+        <v>6.743602641799592</v>
       </c>
       <c r="G54" t="n">
-        <v>674.0966184177332</v>
+        <v>527.0375239137037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Everything has been updated/cleaned up.
</commit_message>
<xml_diff>
--- a/heliostrome/jip_project/results/test_results_Bangladesh.xlsx
+++ b/heliostrome/jip_project/results/test_results_Bangladesh.xlsx
@@ -2677,10 +2677,10 @@
         <v>522</v>
       </c>
       <c r="F44" t="n">
-        <v>10.98050787905975</v>
+        <v>10.36888728709724</v>
       </c>
       <c r="G44" t="n">
-        <v>789.0064062777657</v>
+        <v>781.2895420347404</v>
       </c>
     </row>
     <row r="45">
@@ -2704,10 +2704,10 @@
         <v>887</v>
       </c>
       <c r="F45" t="n">
-        <v>11.02363371829305</v>
+        <v>10.41000634184312</v>
       </c>
       <c r="G45" t="n">
-        <v>759.754732053014</v>
+        <v>753.3783713455551</v>
       </c>
     </row>
     <row r="46">
@@ -2731,10 +2731,10 @@
         <v>1253</v>
       </c>
       <c r="F46" t="n">
-        <v>11.07063181320648</v>
+        <v>10.45509200651106</v>
       </c>
       <c r="G46" t="n">
-        <v>774.2887670850631</v>
+        <v>764.9391393697578</v>
       </c>
     </row>
     <row r="47">

</xml_diff>